<commit_message>
added motor control file
</commit_message>
<xml_diff>
--- a/Documentation/Cost/Cost of items.xlsx
+++ b/Documentation/Cost/Cost of items.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B40)</f>
-        <v>467</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
       </c>
       <c r="F3">
         <f>F2/6</f>
-        <v>77.833333333333329</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
added cost of items
</commit_message>
<xml_diff>
--- a/Documentation/Cost/Cost of items.xlsx
+++ b/Documentation/Cost/Cost of items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Item</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Marko</t>
   </si>
   <si>
-    <t>Raspberry</t>
-  </si>
-  <si>
     <t>12V 2A power supply</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>motor drivers</t>
   </si>
   <si>
-    <t>heat sinks</t>
-  </si>
-  <si>
     <t>ultrasonic sensors</t>
   </si>
   <si>
@@ -86,10 +80,193 @@
     <t>pi camera</t>
   </si>
   <si>
-    <t>SD card</t>
-  </si>
-  <si>
-    <t>drive train materials</t>
+    <t>Screws and L brackets</t>
+  </si>
+  <si>
+    <t>set screws</t>
+  </si>
+  <si>
+    <t>Wheels</t>
+  </si>
+  <si>
+    <t>Wheel</t>
+  </si>
+  <si>
+    <t>L brackets</t>
+  </si>
+  <si>
+    <t>superglue and plastic box (POC)</t>
+  </si>
+  <si>
+    <t>POC wheels, nuts, screws, l brackets</t>
+  </si>
+  <si>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>3/8 nuts, bolts</t>
+  </si>
+  <si>
+    <t>POC wheels v2 and nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC shaft supports </t>
+  </si>
+  <si>
+    <t>Raspberry and SD card</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Sep 29,2017</t>
+  </si>
+  <si>
+    <t>Oct 6,2017</t>
+  </si>
+  <si>
+    <t>Oct 5,2017</t>
+  </si>
+  <si>
+    <t>Oct 4,2017</t>
+  </si>
+  <si>
+    <t>Oct 16,2017</t>
+  </si>
+  <si>
+    <t>Oct 11,2017</t>
+  </si>
+  <si>
+    <t>Oct 12,2017</t>
+  </si>
+  <si>
+    <t>Oct 8,2017</t>
+  </si>
+  <si>
+    <t>5mm rubber pipe for rigid couplings</t>
+  </si>
+  <si>
+    <t>Nov 14,2017</t>
+  </si>
+  <si>
+    <t>Stepper motor driver</t>
+  </si>
+  <si>
+    <t>Nov 13,2017</t>
+  </si>
+  <si>
+    <t>POC 12V battery pack</t>
+  </si>
+  <si>
+    <t>Nov 9,2017</t>
+  </si>
+  <si>
+    <t>Flex couplings</t>
+  </si>
+  <si>
+    <t>Nov 4,2017</t>
+  </si>
+  <si>
+    <t>H bridge</t>
+  </si>
+  <si>
+    <t>Nov 30,2017</t>
+  </si>
+  <si>
+    <t>Drill motors</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Raspberry pi</t>
+  </si>
+  <si>
+    <t>Mar 14,2018</t>
+  </si>
+  <si>
+    <t>16Gb Micro SD card</t>
+  </si>
+  <si>
+    <t>32GB Micro SD Card</t>
+  </si>
+  <si>
+    <t>Jan 31,2018</t>
+  </si>
+  <si>
+    <t>Chain link connectors</t>
+  </si>
+  <si>
+    <t>jan 19,2018</t>
+  </si>
+  <si>
+    <t>Chain and chain breaker</t>
+  </si>
+  <si>
+    <t>Jan 17,2018</t>
+  </si>
+  <si>
+    <t>3 rolls of 3D filament</t>
+  </si>
+  <si>
+    <t>Sprockets</t>
+  </si>
+  <si>
+    <t>Feb 27,2018</t>
+  </si>
+  <si>
+    <t>Couplings (robot shop)</t>
+  </si>
+  <si>
+    <t>Ball bearings</t>
+  </si>
+  <si>
+    <t>Dec 18,2017</t>
+  </si>
+  <si>
+    <t>Dec 9,2017</t>
+  </si>
+  <si>
+    <t>Shaft coupling and optical encoder</t>
+  </si>
+  <si>
+    <t>Poly carbonate</t>
+  </si>
+  <si>
+    <t>Nov 11,2017</t>
+  </si>
+  <si>
+    <t>jan 15,2017</t>
+  </si>
+  <si>
+    <t>Jan 29,2018</t>
+  </si>
+  <si>
+    <t>Jan 18,2018</t>
+  </si>
+  <si>
+    <t>Jan 10,2018</t>
+  </si>
+  <si>
+    <t>Jan 16,2018</t>
+  </si>
+  <si>
+    <t>Jan 22,2018</t>
+  </si>
+  <si>
+    <t>Oct 13,2017</t>
+  </si>
+  <si>
+    <t>Nov,15,2017</t>
+  </si>
+  <si>
+    <t>Jan 12,2018</t>
+  </si>
+  <si>
+    <t>POC wheels first batch</t>
   </si>
 </sst>
 </file>
@@ -133,9 +310,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,16 +630,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -473,195 +654,652 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>12.99</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2">
-        <f>SUM(B2:B40)</f>
-        <v>486</v>
+        <f>SUM(B2:B406)</f>
+        <v>1580.98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>71.3</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3">
         <f>F2/6</f>
-        <v>81</v>
+        <v>263.49666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>13.99</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>41</v>
+        <v>41.8</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>19.98</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>10.99</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>10.73</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>28</v>
+        <v>28.27</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>38</v>
+        <v>18.96</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>13.86</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>37.979999999999997</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>38</v>
+        <v>35.020000000000003</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>35</v>
+        <v>68.84</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>17.48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
-        <v>135</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
+      <c r="B18">
+        <v>10.72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>44.75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>25.96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>130.19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>5.31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>3.94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>29.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25">
+        <v>64.55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>11.57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>11.5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>9.48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>46.99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>10.73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32">
+        <v>34.590000000000003</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>48.67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35">
+        <v>10.99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36">
+        <v>14.99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>29.97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38">
+        <v>4.46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39">
+        <v>50.61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41">
+        <v>51.75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>15.39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44">
+        <v>15.81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45">
+        <v>31.83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46">
+        <v>168.79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding update cost information
</commit_message>
<xml_diff>
--- a/Documentation/Cost/Cost of items.xlsx
+++ b/Documentation/Cost/Cost of items.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSBLH\Documents\GitHub\Capstone\Documentation\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtm\Desktop\Capstone\Documentation\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA4B5F2-2C0E-4F23-9CD4-BECBBEFDD843}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Marko" sheetId="1" r:id="rId1"/>
+    <sheet name="Curtis" sheetId="2" r:id="rId2"/>
+    <sheet name="Alex" sheetId="3" r:id="rId3"/>
+    <sheet name="Keyur" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="105">
   <si>
     <t>Item</t>
   </si>
@@ -267,12 +271,84 @@
   </si>
   <si>
     <t>POC wheels first batch</t>
+  </si>
+  <si>
+    <t>3x Encoders</t>
+  </si>
+  <si>
+    <t>Curtis</t>
+  </si>
+  <si>
+    <t>Flex Cable, Camera extension line, 100cm</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3 Model B Motherboard</t>
+  </si>
+  <si>
+    <t>MALIDA Tee 3/8" x 3/8" x 3/8" quick connect for RO water system (5 pack)</t>
+  </si>
+  <si>
+    <t>Battery for pi</t>
+  </si>
+  <si>
+    <t>Generic Push in Quick Touch to Connect Fitting 1/4"</t>
+  </si>
+  <si>
+    <t>Bread board/ wires</t>
+  </si>
+  <si>
+    <t>20 AWG 300V coper Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Pumps </t>
+  </si>
+  <si>
+    <t>MOSFETs</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4" Tubing </t>
+  </si>
+  <si>
+    <t>temperature sensor waterproof probe wirre</t>
+  </si>
+  <si>
+    <t>Weight Sensors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Cell amplifier </t>
+  </si>
+  <si>
+    <t>MDF Board</t>
+  </si>
+  <si>
+    <t>Robot Shop Couplers</t>
+  </si>
+  <si>
+    <t>1/22/18</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Set Screws</t>
+  </si>
+  <si>
+    <t>Keyur</t>
+  </si>
+  <si>
+    <t>Canadian Tire Stuff</t>
+  </si>
+  <si>
+    <t>Mar 16,2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,12 +386,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,22 +712,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +741,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -676,10 +759,10 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B406)</f>
-        <v>1580.98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1731.6200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -697,10 +780,10 @@
       </c>
       <c r="F3">
         <f>F2/6</f>
-        <v>263.49666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>288.60333333333335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -714,7 +797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -728,7 +811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -742,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -756,7 +839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -770,7 +853,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -784,7 +867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -798,7 +881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -812,7 +895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -826,7 +909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -840,7 +923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -854,7 +937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -868,7 +951,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -882,7 +965,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -896,7 +979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -910,7 +993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -924,7 +1007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -938,7 +1021,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -952,7 +1035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -966,7 +1049,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -980,7 +1063,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -994,7 +1077,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1008,7 +1091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1022,7 +1105,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1119,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1050,7 +1133,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1064,7 +1147,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1078,7 +1161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1092,7 +1175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1106,7 +1189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1120,12 +1203,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
       <c r="B34">
-        <v>48.67</v>
+        <f>48.67*2</f>
+        <v>97.34</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1134,7 +1218,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1148,7 +1232,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1162,7 +1246,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1176,7 +1260,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -1190,7 +1274,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -1204,7 +1288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -1218,7 +1302,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>62</v>
       </c>
@@ -1232,7 +1316,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -1246,7 +1330,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -1260,7 +1344,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1274,7 +1358,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -1288,7 +1372,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -1300,10 +1384,519 @@
       </c>
       <c r="D46" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>67.98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>33.99</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BBB888-2F0F-4818-9F22-BD16AA0CEFF6}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="A1:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43176</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:B406)</f>
+        <v>420.65000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <v>13.98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>F2/6</f>
+        <v>70.108333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4">
+        <v>55.21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43056</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43030</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11">
+        <v>29.04</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12">
+        <v>8.68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>20.77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>6.8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43050</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="2">
+        <v>43041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16">
+        <v>53.17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="2">
+        <v>43149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D57B73-1276-4DEA-B249-CA31E0641BAE}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>45.8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:B406)</f>
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>F2/6</f>
+        <v>7.6333333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E09387A-278B-4B9B-B477-4C9543D2E8CF}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2">
+        <v>12.62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:B406)</f>
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>F2/6</f>
+        <v>2.1033333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>